<commit_message>
Changing stimulus by images and updating conditions file
</commit_message>
<xml_diff>
--- a/experiment/common/conditions.xlsx
+++ b/experiment/common/conditions.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JARS\BCI\common\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8832" windowHeight="8484"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8835" windowHeight="8490"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>condition</t>
   </si>
   <si>
-    <t>ori</t>
-  </si>
-  <si>
     <t>exec_left</t>
   </si>
   <si>
@@ -50,10 +42,19 @@
     <t>img</t>
   </si>
   <si>
-    <t>common/red.png</t>
-  </si>
-  <si>
-    <t>common/white.png</t>
+    <t>common/recall_cross_EL.png</t>
+  </si>
+  <si>
+    <t>common/recall_cross_ER.png</t>
+  </si>
+  <si>
+    <t>common/recall_cross_IL.png</t>
+  </si>
+  <si>
+    <t>common/recall_cross_IR.png</t>
+  </si>
+  <si>
+    <t>common/recall_cross_IT.png</t>
   </si>
 </sst>
 </file>
@@ -89,8 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,7 +365,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -374,78 +376,65 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="55.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
       <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>270</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>